<commit_message>
update score nearby the put_down spot but fail
</commit_message>
<xml_diff>
--- a/ScoreData.xlsx
+++ b/ScoreData.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\PigeonSH\CS\Omok\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D55523FB-715B-4A1B-88EA-A69EC674D2EA}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{10524491-8C9B-47E4-83CB-14D4A6CA55EB}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="4308" yWindow="984" windowWidth="11304" windowHeight="10884" xr2:uid="{C84D99CA-C1E1-4E7F-B26C-261BF3BDF2CD}"/>
   </bookViews>
@@ -34,7 +34,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="37" uniqueCount="35">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="34" uniqueCount="34">
   <si>
     <t>BBBBBB</t>
     <phoneticPr fontId="1" type="noConversion"/>
@@ -49,10 +49,6 @@
   </si>
   <si>
     <t>열린삼</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>이김</t>
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
   <si>
@@ -539,9 +535,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{70CD3BC1-43F2-41CE-BD4A-9FE2D2728473}">
   <dimension ref="A1:G14"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="F8" sqref="F8"/>
-    </sheetView>
+    <sheetView tabSelected="1" workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="17.399999999999999" x14ac:dyDescent="0.4"/>
   <cols>
@@ -551,10 +545,10 @@
   <sheetData>
     <row r="1" spans="1:7" x14ac:dyDescent="0.4">
       <c r="A1" t="s">
-        <v>5</v>
-      </c>
-      <c r="B1" t="s">
         <v>4</v>
+      </c>
+      <c r="B1">
+        <v>10000</v>
       </c>
       <c r="C1">
         <v>6</v>
@@ -563,46 +557,46 @@
         <v>0</v>
       </c>
       <c r="E1" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
     </row>
     <row r="2" spans="1:7" x14ac:dyDescent="0.4">
       <c r="A2" t="s">
         <v>1</v>
       </c>
-      <c r="B2" t="s">
-        <v>4</v>
+      <c r="B2">
+        <v>10000</v>
       </c>
       <c r="C2">
         <v>5</v>
       </c>
       <c r="D2" t="s">
+        <v>14</v>
+      </c>
+      <c r="E2" t="s">
         <v>15</v>
-      </c>
-      <c r="E2" t="s">
-        <v>16</v>
       </c>
     </row>
     <row r="3" spans="1:7" x14ac:dyDescent="0.4">
       <c r="A3" t="s">
         <v>2</v>
       </c>
-      <c r="B3" t="s">
-        <v>4</v>
+      <c r="B3">
+        <v>10000</v>
       </c>
       <c r="C3">
         <v>6</v>
       </c>
       <c r="D3" t="s">
+        <v>16</v>
+      </c>
+      <c r="E3" t="s">
         <v>17</v>
-      </c>
-      <c r="E3" t="s">
-        <v>18</v>
       </c>
     </row>
     <row r="4" spans="1:7" x14ac:dyDescent="0.4">
       <c r="A4" t="s">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="B4">
         <v>1000</v>
@@ -611,16 +605,16 @@
         <v>6</v>
       </c>
       <c r="D4" t="s">
+        <v>18</v>
+      </c>
+      <c r="E4" t="s">
         <v>19</v>
       </c>
-      <c r="E4" t="s">
+      <c r="F4" t="s">
         <v>20</v>
       </c>
-      <c r="F4" t="s">
+      <c r="G4" t="s">
         <v>21</v>
-      </c>
-      <c r="G4" t="s">
-        <v>22</v>
       </c>
     </row>
     <row r="5" spans="1:7" x14ac:dyDescent="0.4">
@@ -634,15 +628,15 @@
         <v>5</v>
       </c>
       <c r="D5" t="s">
+        <v>22</v>
+      </c>
+      <c r="E5" t="s">
         <v>23</v>
-      </c>
-      <c r="E5" t="s">
-        <v>24</v>
       </c>
     </row>
     <row r="6" spans="1:7" x14ac:dyDescent="0.4">
       <c r="A6" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
       <c r="B6">
         <v>800</v>
@@ -651,21 +645,21 @@
         <v>7</v>
       </c>
       <c r="D6" t="s">
+        <v>25</v>
+      </c>
+      <c r="E6" t="s">
+        <v>27</v>
+      </c>
+      <c r="F6" t="s">
         <v>26</v>
       </c>
-      <c r="E6" t="s">
+      <c r="G6" t="s">
         <v>28</v>
-      </c>
-      <c r="F6" t="s">
-        <v>27</v>
-      </c>
-      <c r="G6" t="s">
-        <v>29</v>
       </c>
     </row>
     <row r="7" spans="1:7" x14ac:dyDescent="0.4">
       <c r="A7" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="B7">
         <v>500</v>
@@ -674,15 +668,15 @@
         <v>7</v>
       </c>
       <c r="D7" t="s">
+        <v>29</v>
+      </c>
+      <c r="E7" t="s">
         <v>30</v>
-      </c>
-      <c r="E7" t="s">
-        <v>31</v>
       </c>
     </row>
     <row r="8" spans="1:7" x14ac:dyDescent="0.4">
       <c r="A8" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
       <c r="B8">
         <v>300</v>
@@ -691,15 +685,15 @@
         <v>7</v>
       </c>
       <c r="D8" t="s">
+        <v>32</v>
+      </c>
+      <c r="E8" t="s">
         <v>33</v>
-      </c>
-      <c r="E8" t="s">
-        <v>34</v>
       </c>
     </row>
     <row r="9" spans="1:7" x14ac:dyDescent="0.4">
       <c r="A9" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="B9">
         <v>300</v>
@@ -710,7 +704,7 @@
     </row>
     <row r="10" spans="1:7" x14ac:dyDescent="0.4">
       <c r="A10" t="s">
-        <v>12</v>
+        <v>11</v>
       </c>
       <c r="B10">
         <v>300</v>
@@ -718,7 +712,7 @@
     </row>
     <row r="11" spans="1:7" x14ac:dyDescent="0.4">
       <c r="A11" t="s">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="B11">
         <v>200</v>
@@ -726,7 +720,7 @@
     </row>
     <row r="12" spans="1:7" x14ac:dyDescent="0.4">
       <c r="A12" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="B12">
         <v>100</v>
@@ -734,7 +728,7 @@
     </row>
     <row r="13" spans="1:7" x14ac:dyDescent="0.4">
       <c r="A13" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
       <c r="B13">
         <v>100</v>
@@ -742,7 +736,7 @@
     </row>
     <row r="14" spans="1:7" x14ac:dyDescent="0.4">
       <c r="A14" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="B14">
         <v>10</v>

</xml_diff>